<commit_message>
fix excels because I had to...
</commit_message>
<xml_diff>
--- a/src/test/resources/import/generic/error-header-blank.xlsx
+++ b/src/test/resources/import/generic/error-header-blank.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21705"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{428E2256-EFCA-4F5E-AB0A-924685BCFC44}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="114" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{413EFDA0-51CD-434D-B130-9F63A62DDD7D}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
   <si>
     <t>First Name</t>
   </si>
@@ -90,9 +90,6 @@
   </si>
   <si>
     <t>IT_IT</t>
-  </si>
-  <si>
-    <t>       </t>
   </si>
   <si>
     <t>Language</t>
@@ -593,7 +590,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{0AE93642-3064-541A-AC2E-D2431B81D913}">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -606,14 +603,11 @@
       <c r="A1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>22</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>23</v>
-      </c>
-      <c r="D1" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -621,10 +615,10 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>25</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
       </c>
       <c r="D2">
         <v>300</v>
@@ -635,10 +629,10 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
       </c>
       <c r="D3">
         <v>45</v>
@@ -649,10 +643,10 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>26</v>
       </c>
       <c r="D4">
         <v>60</v>
@@ -663,7 +657,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -677,7 +671,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -688,7 +682,7 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
@@ -702,10 +696,10 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8">
         <v>55</v>

</xml_diff>

<commit_message>
fix after rebase because I accepted wrong xlsx file
well, it's not easy to ready binary files...
</commit_message>
<xml_diff>
--- a/src/test/resources/import/generic/error-header-blank.xlsx
+++ b/src/test/resources/import/generic/error-header-blank.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21705"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="114" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{413EFDA0-51CD-434D-B130-9F63A62DDD7D}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{7E500EC3-3B61-4EAD-BB27-C147927A3CF6}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="31">
   <si>
     <t>First Name</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>IT_IT</t>
+  </si>
+  <si>
+    <t>       </t>
   </si>
   <si>
     <t>Language</t>
@@ -590,7 +593,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{0AE93642-3064-541A-AC2E-D2431B81D913}">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -603,11 +606,14 @@
       <c r="A1" t="s">
         <v>2</v>
       </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
       <c r="C1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -615,10 +621,10 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2">
         <v>300</v>
@@ -629,10 +635,10 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D3">
         <v>45</v>
@@ -643,10 +649,10 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D4">
         <v>60</v>
@@ -657,7 +663,7 @@
         <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>7</v>
@@ -671,7 +677,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
         <v>7</v>
@@ -682,7 +688,7 @@
         <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C7" t="s">
         <v>14</v>
@@ -696,10 +702,10 @@
         <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="D8">
         <v>55</v>

</xml_diff>